<commit_message>
furthering Contexts.adl after merging with origin
</commit_message>
<xml_diff>
--- a/AmpersandData/FormalAmpersand/ContextsTry.xlsx
+++ b/AmpersandData/FormalAmpersand/ContextsTry.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="390" yWindow="510" windowWidth="19815" windowHeight="6855" tabRatio="830" firstSheet="3" activeTab="16"/>
+    <workbookView xWindow="390" yWindow="510" windowWidth="19815" windowHeight="6855" tabRatio="830" firstSheet="3" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="Concept" sheetId="2" r:id="rId1"/>
@@ -14,23 +14,21 @@
     <sheet name="Relation" sheetId="6" r:id="rId5"/>
     <sheet name="Rule" sheetId="7" r:id="rId6"/>
     <sheet name="Signature" sheetId="9" r:id="rId7"/>
-    <sheet name="concs" sheetId="11" r:id="rId8"/>
-    <sheet name="declaredthrough" sheetId="13" r:id="rId9"/>
-    <sheet name="decmean" sheetId="14" r:id="rId10"/>
-    <sheet name="decpurpose" sheetId="15" r:id="rId11"/>
-    <sheet name="gens" sheetId="16" r:id="rId12"/>
-    <sheet name="patterns" sheetId="17" r:id="rId13"/>
-    <sheet name="rrmean" sheetId="19" r:id="rId14"/>
-    <sheet name="rrpurpose" sheetId="20" r:id="rId15"/>
-    <sheet name="usedIn" sheetId="21" r:id="rId16"/>
-    <sheet name="valid" sheetId="22" r:id="rId17"/>
+    <sheet name="declaredthrough" sheetId="13" r:id="rId8"/>
+    <sheet name="decmean" sheetId="14" r:id="rId9"/>
+    <sheet name="decpurpose" sheetId="15" r:id="rId10"/>
+    <sheet name="gens" sheetId="16" r:id="rId11"/>
+    <sheet name="rrmean" sheetId="19" r:id="rId12"/>
+    <sheet name="rrpurpose" sheetId="20" r:id="rId13"/>
+    <sheet name="usedIn" sheetId="21" r:id="rId14"/>
+    <sheet name="valid" sheetId="22" r:id="rId15"/>
   </sheets>
   <calcPr calcId="0" concurrentCalc="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="108" uniqueCount="55">
   <si>
     <t>Concept</t>
   </si>
@@ -107,9 +105,6 @@
     <t>[Signature]</t>
   </si>
   <si>
-    <t>concs</t>
-  </si>
-  <si>
     <t>declaredIn</t>
   </si>
   <si>
@@ -143,9 +138,6 @@
     <t>name</t>
   </si>
   <si>
-    <t>patterns</t>
-  </si>
-  <si>
     <t>rrmean</t>
   </si>
   <si>
@@ -158,9 +150,6 @@
     <t>src</t>
   </si>
   <si>
-    <t>term</t>
-  </si>
-  <si>
     <t>tgt</t>
   </si>
   <si>
@@ -185,18 +174,12 @@
     <t>r</t>
   </si>
   <si>
-    <t>relations~</t>
-  </si>
-  <si>
     <t>A*B</t>
   </si>
   <si>
     <t>Pat2</t>
   </si>
   <si>
-    <t>declarations~</t>
-  </si>
-  <si>
     <t>rel</t>
   </si>
   <si>
@@ -204,6 +187,12 @@
   </si>
   <si>
     <t>Pattern2</t>
+  </si>
+  <si>
+    <t>formalExpression</t>
+  </si>
+  <si>
+    <t>uses~</t>
   </si>
 </sst>
 </file>
@@ -555,7 +544,7 @@
         <v>17</v>
       </c>
       <c r="B1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
@@ -568,18 +557,18 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="B3" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="B4" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
     </row>
   </sheetData>
@@ -600,7 +589,7 @@
         <v>22</v>
       </c>
       <c r="B1" t="s">
-        <v>28</v>
+        <v>31</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
@@ -608,6 +597,64 @@
         <v>12</v>
       </c>
       <c r="B2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B1" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>23</v>
+      </c>
+      <c r="B1" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>13</v>
+      </c>
+      <c r="B2" t="s">
         <v>6</v>
       </c>
     </row>
@@ -616,7 +663,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B2"/>
   <sheetViews>
@@ -626,10 +673,39 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>23</v>
+      </c>
+      <c r="B1" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>13</v>
+      </c>
+      <c r="B2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
         <v>22</v>
       </c>
       <c r="B1" t="s">
-        <v>32</v>
+        <v>41</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
@@ -637,15 +713,15 @@
         <v>12</v>
       </c>
       <c r="B2" t="s">
-        <v>11</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+        <v>3</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B2"/>
   <sheetViews>
@@ -655,173 +731,10 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>18</v>
-      </c>
-      <c r="B1" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>1</v>
-      </c>
-      <c r="B2" t="s">
-        <v>4</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B4"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>18</v>
-      </c>
-      <c r="B1" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>1</v>
-      </c>
-      <c r="B2" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>48</v>
-      </c>
-      <c r="B3" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>48</v>
-      </c>
-      <c r="B4" t="s">
-        <v>53</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
         <v>23</v>
       </c>
       <c r="B1" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>13</v>
-      </c>
-      <c r="B2" t="s">
-        <v>6</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>23</v>
-      </c>
-      <c r="B1" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>13</v>
-      </c>
-      <c r="B2" t="s">
-        <v>11</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>22</v>
-      </c>
-      <c r="B1" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>12</v>
-      </c>
-      <c r="B2" t="s">
-        <v>3</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B2"/>
-  <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>23</v>
-      </c>
-      <c r="B1" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
@@ -852,7 +765,7 @@
         <v>18</v>
       </c>
       <c r="B1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
@@ -865,10 +778,10 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="B3" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
     </row>
   </sheetData>
@@ -889,10 +802,10 @@
         <v>19</v>
       </c>
       <c r="B1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
@@ -913,44 +826,56 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B4"/>
+  <dimension ref="A1:C4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>20</v>
       </c>
       <c r="B1" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+        <v>35</v>
+      </c>
+      <c r="C1" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>7</v>
       </c>
       <c r="B2" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C2" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
+        <v>46</v>
+      </c>
+      <c r="B3" t="s">
+        <v>51</v>
+      </c>
+      <c r="C3" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
         <v>49</v>
       </c>
-      <c r="B3" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>53</v>
-      </c>
       <c r="B4" t="s">
-        <v>57</v>
+        <v>52</v>
+      </c>
+      <c r="C4" t="s">
+        <v>45</v>
       </c>
     </row>
   </sheetData>
@@ -963,7 +888,7 @@
   <dimension ref="A1:H4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+      <selection activeCell="G7" sqref="G7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -973,13 +898,13 @@
         <v>22</v>
       </c>
       <c r="B1" t="s">
-        <v>51</v>
+        <v>35</v>
       </c>
       <c r="C1" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="D1" t="s">
-        <v>40</v>
+        <v>28</v>
       </c>
       <c r="E1" t="s">
         <v>29</v>
@@ -988,10 +913,10 @@
         <v>30</v>
       </c>
       <c r="G1" t="s">
-        <v>31</v>
+        <v>25</v>
       </c>
       <c r="H1" t="s">
-        <v>54</v>
+        <v>25</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
@@ -999,13 +924,13 @@
         <v>12</v>
       </c>
       <c r="B2" t="s">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="C2" t="s">
-        <v>5</v>
+        <v>15</v>
       </c>
       <c r="D2" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="E2" t="s">
         <v>16</v>
@@ -1014,109 +939,115 @@
         <v>16</v>
       </c>
       <c r="G2" t="s">
-        <v>16</v>
+        <v>7</v>
       </c>
       <c r="H2" t="s">
-        <v>7</v>
+        <v>1</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
+        <v>47</v>
+      </c>
+      <c r="B3" t="s">
         <v>50</v>
       </c>
-      <c r="B3" t="s">
+      <c r="C3" t="s">
         <v>48</v>
       </c>
-      <c r="C3" t="s">
-        <v>55</v>
-      </c>
-      <c r="D3" t="s">
-        <v>52</v>
+      <c r="G3" t="s">
+        <v>46</v>
       </c>
       <c r="H3" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>50</v>
-      </c>
-      <c r="H4" t="s">
+        <v>47</v>
+      </c>
+      <c r="G4" t="s">
+        <v>49</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:F2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F3" sqref="F3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>23</v>
+      </c>
+      <c r="B1" t="s">
+        <v>35</v>
+      </c>
+      <c r="C1" t="s">
+        <v>38</v>
+      </c>
+      <c r="D1" t="s">
         <v>53</v>
       </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>23</v>
-      </c>
-      <c r="B1" t="s">
-        <v>36</v>
+      <c r="E1" t="s">
+        <v>25</v>
+      </c>
+      <c r="F1" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>13</v>
+      </c>
+      <c r="B2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C2" t="s">
+        <v>15</v>
+      </c>
+      <c r="D2" t="s">
+        <v>3</v>
+      </c>
+      <c r="E2" t="s">
+        <v>7</v>
+      </c>
+      <c r="F2" t="s">
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>24</v>
+      </c>
+      <c r="B1" t="s">
+        <v>39</v>
       </c>
       <c r="C1" t="s">
         <v>40</v>
       </c>
-      <c r="D1" t="s">
-        <v>42</v>
-      </c>
-      <c r="E1" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>13</v>
-      </c>
-      <c r="B2" t="s">
-        <v>14</v>
-      </c>
-      <c r="C2" t="s">
-        <v>15</v>
-      </c>
-      <c r="D2" t="s">
-        <v>3</v>
-      </c>
-      <c r="E2" t="s">
-        <v>7</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C3"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>24</v>
-      </c>
-      <c r="B1" t="s">
-        <v>41</v>
-      </c>
-      <c r="C1" t="s">
-        <v>43</v>
-      </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
@@ -1131,13 +1062,13 @@
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="B3" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="C3" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
     </row>
   </sheetData>
@@ -1149,26 +1080,24 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3:B4"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>18</v>
-      </c>
-      <c r="B1" t="s">
-        <v>25</v>
+        <v>21</v>
+      </c>
+      <c r="B1" t="s">
+        <v>26</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>1</v>
-      </c>
-      <c r="B2" t="s">
-        <v>0</v>
+        <v>10</v>
+      </c>
+      <c r="B2" t="s">
+        <v>9</v>
       </c>
     </row>
   </sheetData>
@@ -1186,7 +1115,7 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="B1" t="s">
         <v>27</v>
@@ -1194,10 +1123,10 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>10</v>
-      </c>
-      <c r="B2" t="s">
-        <v>9</v>
+        <v>12</v>
+      </c>
+      <c r="B2" t="s">
+        <v>6</v>
       </c>
     </row>
   </sheetData>

</xml_diff>